<commit_message>
organinzed the csv files
</commit_message>
<xml_diff>
--- a/src/ColonyCounter/summary_results.xlsx
+++ b/src/ColonyCounter/summary_results.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="IMG_5297.JPG" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="IMG_5265.jpg" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="IMG_5297.JPG1" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -767,7 +769,6 @@
       <c r="E2" t="n">
         <v>912.119</v>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -791,7 +792,6 @@
       <c r="E3" t="n">
         <v>276.432</v>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -972,6 +972,228 @@
         <v>276.432</v>
       </c>
       <c r="F10" t="n">
+        <v>189.652</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>project_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>image_file_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>colony_label</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_colonies</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>average_size</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>std_dev_size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IMG_5264.jpg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Kbd17-1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>115</v>
+      </c>
+      <c r="E2" t="n">
+        <v>944.1130000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>463.726</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IMG_5265.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kbd17-2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E3" t="n">
+        <v>685.158</v>
+      </c>
+      <c r="F3" t="n">
+        <v>464.293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>project_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>image_file_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>colony_label</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_colonies</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>average_size</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>std_dev_size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IMG_5264.jpg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Kbd17-1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>115</v>
+      </c>
+      <c r="E2" t="n">
+        <v>944.1130000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>463.726</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IMG_5265.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kbd17-2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E3" t="n">
+        <v>685.158</v>
+      </c>
+      <c r="F3" t="n">
+        <v>464.293</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IMG_5297.JPG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kbd5-2</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1277</v>
+      </c>
+      <c r="E4" t="n">
+        <v>276.432</v>
+      </c>
+      <c r="F4" t="n">
         <v>189.652</v>
       </c>
     </row>

</xml_diff>